<commit_message>
improve xlsx template for showing VAT amount
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A125D79E-7510-A746-B865-75E64DDAD9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A32D66-D912-874D-B946-736634C3130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11011,7 +11011,7 @@
     <definedName name="zer" hidden="1">{#N/A,#N/A,FALSE,"Calc";#N/A,#N/A,FALSE,"Sensitivity";#N/A,#N/A,FALSE,"LT Earn.Dil.";#N/A,#N/A,FALSE,"Dil. AVP"}</definedName>
     <definedName name="ZERTRET" hidden="1">#REF!</definedName>
     <definedName name="zezrzrzerz" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$63</definedName>
     <definedName name="zz" hidden="1">{"MARCH",#N/A,FALSE,"CONSO OPEX 5899";"FullOpex",#N/A,FALSE,"CONSO OPEX 5899"}</definedName>
     <definedName name="ZZZ" hidden="1">{#N/A,#N/A,TRUE,"Total Market";#N/A,#N/A,TRUE,"Pricing Table";#N/A,#N/A,TRUE,"Residential Minutes";#N/A,#N/A,TRUE,"Small Bus Minutes";#N/A,#N/A,TRUE,"Medium Bus Minures";#N/A,#N/A,TRUE,"Corporate Min penetration";#N/A,#N/A,TRUE,"Line Penetration";#N/A,#N/A,TRUE,"Direct Line Penetration";#N/A,#N/A,TRUE,"Indirect Lines";#N/A,#N/A,TRUE,"Penetration% by Customer";#N/A,#N/A,TRUE,"Penetration% by Product";#N/A,#N/A,TRUE,"Minutes-Revenue by Product";#N/A,#N/A,TRUE,"Product Minute penetration";#N/A,#N/A,TRUE,"Customer Minutes Penetration"}</definedName>
     <definedName name="ZZZA" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps";"debt comps",#N/A,FALSE,"CS Comps";"debt comps",#N/A,FALSE,"PS Comps";"debt comps",#N/A,FALSE,"GIC_Comps";"debt comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
@@ -11446,12 +11446,6 @@
       <name val="Helvetica 55 Roman"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="12"/>
@@ -11478,6 +11472,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF9B9B9B"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -11957,7 +11959,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -12066,9 +12068,6 @@
     <xf numFmtId="165" fontId="22" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="38" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="26" borderId="17" xfId="30" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -12101,7 +12100,7 @@
     <xf numFmtId="165" fontId="27" fillId="24" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="38" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="27" fillId="24" borderId="12" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12119,9 +12118,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="47" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -12169,7 +12168,7 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="41" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="40" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -12221,6 +12220,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="165" fontId="43" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12275,15 +12277,6 @@
     <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="3" fillId="24" borderId="11" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -12319,6 +12312,15 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -12751,10 +12753,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13340,7 +13342,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="65"/>
+      <c r="A1" s="64"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -13352,21 +13354,21 @@
       <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="20">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="129"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="141"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="66"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -13378,102 +13380,102 @@
       <c r="J3" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="14">
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="99" t="s">
+      <c r="E5" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="100"/>
-      <c r="G5" s="130">
+      <c r="F5" s="99"/>
+      <c r="G5" s="127">
         <f ca="1">NOW()</f>
-        <v>45194.744169560188</v>
+        <v>45196.822879976855</v>
       </c>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="128"/>
     </row>
     <row r="6" spans="1:10" ht="55" customHeight="1">
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="98"/>
-      <c r="J6" s="102"/>
+      <c r="F6" s="97"/>
+      <c r="J6" s="101"/>
     </row>
     <row r="7" spans="1:10" ht="14">
-      <c r="A7" s="75"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="68" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="E7" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="133"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="130"/>
     </row>
     <row r="8" spans="1:10" ht="14">
-      <c r="C8" s="68">
+      <c r="C8" s="67">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A9" s="134" t="s">
+      <c r="A9" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="69" t="s">
+      <c r="B9" s="132"/>
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="J9" s="135"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="132"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="89">
+      <c r="B10" s="61"/>
+      <c r="C10" s="88">
         <v>10</v>
       </c>
-      <c r="D10" s="137" t="s">
+      <c r="D10" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="138"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="139"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="136"/>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="38"/>
-      <c r="C11" s="89">
+      <c r="C11" s="88">
         <v>250</v>
       </c>
-      <c r="D11" s="140"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="141"/>
-      <c r="G11" s="141"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
       <c r="H11" s="39"/>
       <c r="J11" s="8"/>
     </row>
@@ -13482,7 +13484,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="41"/>
-      <c r="C12" s="89">
+      <c r="C12" s="88">
         <v>0</v>
       </c>
       <c r="D12" s="125"/>
@@ -13498,7 +13500,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="16"/>
-      <c r="C13" s="89">
+      <c r="C13" s="88">
         <v>12</v>
       </c>
       <c r="D13" s="113"/>
@@ -13516,7 +13518,7 @@
       <c r="B15" s="121"/>
       <c r="C15" s="121"/>
       <c r="D15" s="122"/>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="49" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="18" t="str">
@@ -13561,34 +13563,34 @@
       <c r="E17" s="33">
         <v>10</v>
       </c>
-      <c r="F17" s="91">
+      <c r="F17" s="90">
         <v>3109</v>
       </c>
       <c r="G17" s="34">
         <v>1</v>
       </c>
-      <c r="H17" s="90">
+      <c r="H17" s="89">
         <v>36</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="62">
         <v>0.15</v>
       </c>
-      <c r="J17" s="64">
+      <c r="J17" s="63">
         <f>F17*G17*(1-I17)</f>
         <v>2642.65</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="48"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A19" s="44"/>
@@ -13604,31 +13606,31 @@
     <row r="20" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="2"/>
-      <c r="D20" s="82" t="s">
+      <c r="D20" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="60">
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="59">
         <f>SUM(J17:J17)</f>
         <v>2642.65</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="D21" s="84" t="str">
+      <c r="D21" s="83" t="str">
         <f>C9&amp;" SUPPORT  ("&amp;C10&amp;"% Minimum " &amp; C11&amp;")"</f>
         <v>BUSINESS SUPPORT  (10% Minimum 250)</v>
       </c>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="46">
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="56">
         <f>MAX(0.01*$C$10*J20,$C$11)</f>
         <v>264.26500000000004</v>
       </c>
@@ -13636,16 +13638,16 @@
     <row r="22" spans="1:10" s="19" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="11"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="84" t="str">
+      <c r="D22" s="83" t="str">
         <f>IF(C12&gt;0,"Exceptional Discount (-"&amp;C12&amp;"%)","")</f>
         <v/>
       </c>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="60">
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="56">
         <f>(0-J20-J21)*($C$12/100)</f>
         <v>0</v>
       </c>
@@ -13654,250 +13656,254 @@
       <c r="A23" s="11"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="84" t="str">
+      <c r="D23" s="83" t="str">
         <f>"MONTHLY COST ex. VAT with SUPPORT in "&amp;C6</f>
         <v>MONTHLY COST ex. VAT with SUPPORT in EURO</v>
       </c>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="59">
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="58">
         <f>J20+J21+J22</f>
         <v>2906.915</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14" customHeight="1">
+    <row r="24" spans="1:10" ht="16" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="84" t="s">
+      <c r="D24" s="83" t="str">
+        <f>"VAT ("&amp;$C$8&amp;"%)"</f>
+        <v>VAT (20%)</v>
+      </c>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="108">
+        <f>$C$8*J23/100</f>
+        <v>581.38300000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" customHeight="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="20">
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="20">
         <f>SUM(E17:E18)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="6" customFormat="1" ht="16" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="D25" s="84" t="str">
+    <row r="26" spans="1:10" ht="14" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="20"/>
+    </row>
+    <row r="27" spans="1:10" s="6" customFormat="1" ht="16" customHeight="1">
+      <c r="A27" s="11"/>
+      <c r="D27" s="83" t="str">
         <f>"Monthly COST including VAT and SUPPORT in "&amp;C6</f>
         <v>Monthly COST including VAT and SUPPORT in EURO</v>
       </c>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="57">
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="56">
         <f>J23*(1+$C$8/100)</f>
         <v>3488.2979999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="D26" s="84" t="str">
+    <row r="28" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
+      <c r="A28" s="11"/>
+      <c r="D28" s="83" t="str">
         <f>"Setup Fees including VAT in "&amp;C6</f>
         <v>Setup Fees including VAT in EURO</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="57">
-        <f>J24*(1+$C$8/100)</f>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="56">
+        <f>J25*(1+$C$8/100)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="D27" s="84" t="str">
+    <row r="29" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
+      <c r="A29" s="11"/>
+      <c r="D29" s="83" t="str">
         <f>"BUDGET in "&amp;C6&amp;" ex. VAT ("&amp;$C$13&amp;" Months)"</f>
         <v>BUDGET in EURO ex. VAT (12 Months)</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="45">
-        <f>J23*$C$13+J24</f>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="45">
+        <f>J23*$C$13+J25</f>
         <v>34892.979999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="6" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="D28" s="87" t="str">
+    <row r="30" spans="1:10" s="6" customFormat="1" ht="15.5" customHeight="1">
+      <c r="A30" s="11"/>
+      <c r="D30" s="86" t="str">
         <f>"BUDGET in "&amp;C6&amp;" including VAT ("&amp;$C$13&amp;" Months) - "&amp;$C$7&amp;" "&amp;$C$8&amp;"%"</f>
         <v>BUDGET in EURO including VAT (12 Months) - TVA 20%</v>
       </c>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="58">
-        <f>J27*1.2</f>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="57">
+        <f>J29*1.2</f>
         <v>41871.575999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14">
-      <c r="A29" s="11"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+    <row r="31" spans="1:10" ht="14">
+      <c r="A31" s="11"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
     </row>
-    <row r="30" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A30" s="47"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
+    <row r="32" spans="1:10" s="6" customFormat="1" ht="14">
+      <c r="A32" s="46"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="4"/>
     </row>
-    <row r="31" spans="1:10" ht="14">
-      <c r="A31" s="27" t="s">
+    <row r="33" spans="1:10" ht="14">
+      <c r="A33" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="29"/>
     </row>
-    <row r="32" spans="1:10" ht="14">
-      <c r="A32" s="111"/>
-      <c r="B32" s="112"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="31"/>
+    <row r="34" spans="1:10" ht="14">
+      <c r="A34" s="111"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
     </row>
-    <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="76"/>
-      <c r="B33" s="76" t="s">
+    <row r="35" spans="1:10" ht="15">
+      <c r="A35" s="75"/>
+      <c r="B35" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C35" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="79"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="78"/>
     </row>
-    <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77" t="s">
+    <row r="36" spans="1:10" ht="15">
+      <c r="A36" s="76"/>
+      <c r="B36" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="78" t="s">
+      <c r="C36" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="79"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="78"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="95"/>
+    <row r="37" spans="1:10">
+      <c r="A37" s="94"/>
     </row>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="92"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="80" t="s">
+    <row r="38" spans="1:10" ht="15">
+      <c r="A38" s="91"/>
+      <c r="B38" s="92"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="85"/>
-    </row>
-    <row r="37" spans="1:10" ht="14">
-      <c r="A37" s="37"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="109"/>
-      <c r="I37" s="109"/>
-      <c r="J37" s="110"/>
-    </row>
-    <row r="38" spans="1:10" ht="14">
-      <c r="A38" s="37"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="109"/>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="110"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="84"/>
     </row>
     <row r="39" spans="1:10" ht="14">
-      <c r="A39" s="35"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
+      <c r="A39" s="37"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="8"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="110"/>
     </row>
     <row r="40" spans="1:10" ht="14">
-      <c r="A40" s="32"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="6"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="8"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
+      <c r="J40" s="110"/>
     </row>
     <row r="41" spans="1:10" ht="14">
-      <c r="A41" s="37"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="39"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="14" t="s">
-        <v>32</v>
+      <c r="C41" s="39"/>
+      <c r="D41" s="11" t="s">
+        <v>31</v>
       </c>
-      <c r="E41" s="17"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -13905,11 +13911,11 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10" ht="14">
-      <c r="A42" s="25"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="17"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -13917,13 +13923,13 @@
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="1:10" ht="14">
-      <c r="A43" s="92"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="11" t="s">
-        <v>33</v>
+      <c r="A43" s="37"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="14" t="s">
+        <v>32</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -13931,11 +13937,11 @@
       <c r="J43" s="8"/>
     </row>
     <row r="44" spans="1:10" ht="14">
-      <c r="A44" s="92"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="6"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -13943,10 +13949,12 @@
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="1:10" ht="14">
-      <c r="A45" s="92"/>
-      <c r="B45" s="93"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="92"/>
       <c r="C45" s="39"/>
-      <c r="D45" s="11"/>
+      <c r="D45" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -13955,8 +13963,8 @@
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="1:10" ht="14">
-      <c r="A46" s="92"/>
-      <c r="B46" s="93"/>
+      <c r="A46" s="91"/>
+      <c r="B46" s="92"/>
       <c r="C46" s="39"/>
       <c r="D46" s="11"/>
       <c r="E46" s="6"/>
@@ -13967,8 +13975,8 @@
       <c r="J46" s="8"/>
     </row>
     <row r="47" spans="1:10" ht="14">
-      <c r="A47" s="92"/>
-      <c r="B47" s="93"/>
+      <c r="A47" s="91"/>
+      <c r="B47" s="92"/>
       <c r="C47" s="39"/>
       <c r="D47" s="11"/>
       <c r="E47" s="6"/>
@@ -13979,109 +13987,123 @@
       <c r="J47" s="8"/>
     </row>
     <row r="48" spans="1:10" ht="14">
-      <c r="A48" s="92"/>
-      <c r="B48" s="93"/>
+      <c r="A48" s="91"/>
+      <c r="B48" s="92"/>
       <c r="C48" s="39"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="96"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="1" t="s">
+    <row r="49" spans="1:10" ht="14">
+      <c r="A49" s="91"/>
+      <c r="B49" s="92"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" ht="14">
+      <c r="A50" s="91"/>
+      <c r="B50" s="92"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="95"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="5"/>
-      <c r="B50" s="26"/>
+    <row r="52" spans="1:10">
+      <c r="A52" s="5"/>
+      <c r="B52" s="26"/>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="5"/>
+    <row r="53" spans="1:10">
+      <c r="A53" s="5"/>
     </row>
-    <row r="52" spans="1:10" ht="21">
-      <c r="A52" s="106" t="s">
+    <row r="54" spans="1:10" ht="21">
+      <c r="A54" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="107"/>
-      <c r="C52" s="108"/>
-      <c r="D52" s="108"/>
-      <c r="E52" s="108"/>
-      <c r="F52" s="108"/>
-      <c r="G52" s="108"/>
-      <c r="H52" s="108"/>
-      <c r="I52" s="108"/>
-      <c r="J52" s="108"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="107"/>
+      <c r="D54" s="107"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="107"/>
+      <c r="G54" s="107"/>
+      <c r="H54" s="107"/>
+      <c r="I54" s="107"/>
+      <c r="J54" s="107"/>
     </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="70" t="s">
+    <row r="55" spans="1:10">
+      <c r="A55" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="43"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="42"/>
-      <c r="C54" s="43"/>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="71"/>
       <c r="B55" s="42"/>
       <c r="C55" s="43"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="72" t="s">
-        <v>41</v>
+      <c r="A56" s="70" t="s">
+        <v>36</v>
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="43"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="74" t="s">
-        <v>40</v>
-      </c>
+      <c r="A57" s="70"/>
       <c r="B57" s="42"/>
       <c r="C57" s="43"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="73" t="s">
-        <v>38</v>
+      <c r="A58" s="71" t="s">
+        <v>41</v>
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="43"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="74" t="s">
-        <v>39</v>
+      <c r="A59" s="73" t="s">
+        <v>40</v>
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="43"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="72"/>
+      <c r="A60" s="72" t="s">
+        <v>38</v>
+      </c>
       <c r="B60" s="42"/>
       <c r="C60" s="43"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="74"/>
+      <c r="A61" s="73" t="s">
+        <v>39</v>
+      </c>
       <c r="B61" s="42"/>
       <c r="C61" s="43"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="73"/>
+      <c r="A62" s="71"/>
       <c r="B62" s="42"/>
       <c r="C62" s="43"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="74"/>
+      <c r="A63" s="73"/>
       <c r="B63" s="42"/>
       <c r="C63" s="43"/>
     </row>
@@ -14091,17 +14113,17 @@
       <c r="C64" s="43"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="74"/>
+      <c r="A65" s="73"/>
       <c r="B65" s="42"/>
       <c r="C65" s="43"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="73"/>
+      <c r="A66" s="71"/>
       <c r="B66" s="42"/>
       <c r="C66" s="43"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="74"/>
+      <c r="A67" s="73"/>
       <c r="B67" s="42"/>
       <c r="C67" s="43"/>
     </row>
@@ -14111,17 +14133,17 @@
       <c r="C68" s="43"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="74"/>
+      <c r="A69" s="73"/>
       <c r="B69" s="42"/>
       <c r="C69" s="43"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="73"/>
+      <c r="A70" s="71"/>
       <c r="B70" s="42"/>
       <c r="C70" s="43"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="74"/>
+      <c r="A71" s="73"/>
       <c r="B71" s="42"/>
       <c r="C71" s="43"/>
     </row>
@@ -14131,17 +14153,17 @@
       <c r="C72" s="43"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="74"/>
+      <c r="A73" s="73"/>
       <c r="B73" s="42"/>
       <c r="C73" s="43"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="73"/>
+      <c r="A74" s="71"/>
       <c r="B74" s="42"/>
       <c r="C74" s="43"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="74"/>
+      <c r="A75" s="73"/>
       <c r="B75" s="42"/>
       <c r="C75" s="43"/>
     </row>
@@ -14151,17 +14173,17 @@
       <c r="C76" s="43"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="74"/>
+      <c r="A77" s="73"/>
       <c r="B77" s="42"/>
       <c r="C77" s="43"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="73"/>
+      <c r="A78" s="71"/>
       <c r="B78" s="42"/>
       <c r="C78" s="43"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="74"/>
+      <c r="A79" s="73"/>
       <c r="B79" s="42"/>
       <c r="C79" s="43"/>
     </row>
@@ -14171,17 +14193,17 @@
       <c r="C80" s="43"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="74"/>
+      <c r="A81" s="73"/>
       <c r="B81" s="42"/>
       <c r="C81" s="43"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="73"/>
+      <c r="A82" s="71"/>
       <c r="B82" s="42"/>
       <c r="C82" s="43"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="74"/>
+      <c r="A83" s="73"/>
       <c r="B83" s="42"/>
       <c r="C83" s="43"/>
     </row>
@@ -14191,17 +14213,17 @@
       <c r="C84" s="43"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="74"/>
+      <c r="A85" s="73"/>
       <c r="B85" s="42"/>
       <c r="C85" s="43"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="73"/>
+      <c r="A86" s="71"/>
       <c r="B86" s="42"/>
       <c r="C86" s="43"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="74"/>
+      <c r="A87" s="73"/>
       <c r="B87" s="42"/>
       <c r="C87" s="43"/>
     </row>
@@ -14211,74 +14233,83 @@
       <c r="C88" s="43"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="74"/>
+      <c r="A89" s="73"/>
+      <c r="B89" s="42"/>
+      <c r="C89" s="43"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="73"/>
+      <c r="A90" s="71"/>
+      <c r="B90" s="42"/>
+      <c r="C90" s="43"/>
     </row>
-    <row r="91" spans="1:3" ht="15" customHeight="1">
-      <c r="A91" s="74"/>
+    <row r="91" spans="1:3">
+      <c r="A91" s="73"/>
     </row>
-    <row r="92" spans="1:3" ht="15" customHeight="1">
+    <row r="92" spans="1:3">
       <c r="A92" s="72"/>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="74"/>
+    <row r="93" spans="1:3" ht="15" customHeight="1">
+      <c r="A93" s="73"/>
     </row>
-    <row r="94" spans="1:3" ht="16" customHeight="1">
-      <c r="A94" s="73"/>
+    <row r="94" spans="1:3" ht="15" customHeight="1">
+      <c r="A94" s="71"/>
     </row>
-    <row r="95" spans="1:3" ht="15" customHeight="1">
-      <c r="A95" s="74"/>
+    <row r="95" spans="1:3">
+      <c r="A95" s="73"/>
     </row>
-    <row r="96" spans="1:3" ht="15" customHeight="1">
+    <row r="96" spans="1:3" ht="16" customHeight="1">
       <c r="A96" s="72"/>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1">
-      <c r="A97" s="74"/>
+      <c r="A97" s="73"/>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1">
-      <c r="A98" s="73"/>
+      <c r="A98" s="71"/>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1">
-      <c r="A99" s="74"/>
+      <c r="A99" s="73"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" ht="15" customHeight="1">
       <c r="A100" s="72"/>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="74"/>
+    <row r="101" spans="1:1" ht="15" customHeight="1">
+      <c r="A101" s="73"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="73"/>
+      <c r="A102" s="71"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="74"/>
+      <c r="A103" s="73"/>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="72"/>
     </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="73"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="71"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A2:J2"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:G11"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G39:J39"/>
     <mergeCell ref="D13:J13"/>
     <mergeCell ref="A16:J16"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
   </mergeCells>
-  <phoneticPr fontId="42" type="noConversion"/>
+  <phoneticPr fontId="41" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A59" r:id="rId1" xr:uid="{B64823B1-50BF-1C44-8515-7EEF2938EDB0}"/>
+    <hyperlink ref="A61" r:id="rId1" xr:uid="{B64823B1-50BF-1C44-8515-7EEF2938EDB0}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fixed BUG PHrase de commit condition > 1 not true
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A32D66-D912-874D-B946-736634C3130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1CFBDC-62E4-9F45-A5F6-0736273C4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="28800" windowHeight="19060" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quote" sheetId="58" r:id="rId1"/>
@@ -10640,6 +10640,7 @@
     <definedName name="Portails" hidden="1">{"' calendrier 2000'!$A$1:$Q$38"}</definedName>
     <definedName name="pp" hidden="1">{#N/A,#N/A,FALSE,"Calc";#N/A,#N/A,FALSE,"Sensitivity";#N/A,#N/A,FALSE,"LT Earn.Dil.";#N/A,#N/A,FALSE,"Dil. AVP"}</definedName>
     <definedName name="Pres" hidden="1">{#N/A,#N/A,TRUE,"Cover sheet";#N/A,#N/A,TRUE,"Summary";#N/A,#N/A,TRUE,"Key Assumptions";#N/A,#N/A,TRUE,"Profit &amp; Loss";#N/A,#N/A,TRUE,"Balance Sheet";#N/A,#N/A,TRUE,"Cashflow";#N/A,#N/A,TRUE,"IRR";#N/A,#N/A,TRUE,"Ratios";#N/A,#N/A,TRUE,"Debt analysis"}</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$37</definedName>
     <definedName name="Print_CSC_Report_2" hidden="1">{"CSC_1",#N/A,FALSE,"CSC Outputs";"CSC_2",#N/A,FALSE,"CSC Outputs"}</definedName>
     <definedName name="Print_CSC_Report_3" hidden="1">{"CSC_1",#N/A,FALSE,"CSC Outputs";"CSC_2",#N/A,FALSE,"CSC Outputs"}</definedName>
     <definedName name="print4" hidden="1">{#N/A,#N/A,FALSE,"Operations";#N/A,#N/A,FALSE,"Financials"}</definedName>
@@ -11011,7 +11012,6 @@
     <definedName name="zer" hidden="1">{#N/A,#N/A,FALSE,"Calc";#N/A,#N/A,FALSE,"Sensitivity";#N/A,#N/A,FALSE,"LT Earn.Dil.";#N/A,#N/A,FALSE,"Dil. AVP"}</definedName>
     <definedName name="ZERTRET" hidden="1">#REF!</definedName>
     <definedName name="zezrzrzerz" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$63</definedName>
     <definedName name="zz" hidden="1">{"MARCH",#N/A,FALSE,"CONSO OPEX 5899";"FullOpex",#N/A,FALSE,"CONSO OPEX 5899"}</definedName>
     <definedName name="ZZZ" hidden="1">{#N/A,#N/A,TRUE,"Total Market";#N/A,#N/A,TRUE,"Pricing Table";#N/A,#N/A,TRUE,"Residential Minutes";#N/A,#N/A,TRUE,"Small Bus Minutes";#N/A,#N/A,TRUE,"Medium Bus Minures";#N/A,#N/A,TRUE,"Corporate Min penetration";#N/A,#N/A,TRUE,"Line Penetration";#N/A,#N/A,TRUE,"Direct Line Penetration";#N/A,#N/A,TRUE,"Indirect Lines";#N/A,#N/A,TRUE,"Penetration% by Customer";#N/A,#N/A,TRUE,"Penetration% by Product";#N/A,#N/A,TRUE,"Minutes-Revenue by Product";#N/A,#N/A,TRUE,"Product Minute penetration";#N/A,#N/A,TRUE,"Customer Minutes Penetration"}</definedName>
     <definedName name="ZZZA" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps";"debt comps",#N/A,FALSE,"CS Comps";"debt comps",#N/A,FALSE,"PS Comps";"debt comps",#N/A,FALSE,"GIC_Comps";"debt comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
@@ -11034,22 +11034,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">Client : </t>
-  </si>
-  <si>
-    <t>Contact :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email : </t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>CLIENT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>BUSINESS</t>
   </si>
@@ -11058,9 +11043,6 @@
   </si>
   <si>
     <t>Zone de Confiance - France - RBX</t>
-  </si>
-  <si>
-    <t>TVA</t>
   </si>
   <si>
     <t>EURO</t>
@@ -11099,94 +11081,128 @@
     <t>QUOTE</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Quote Number</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For the attention of : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone : </t>
-  </si>
-  <si>
-    <t>Setup Fee</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Commitment duration (Month)</t>
-  </si>
-  <si>
-    <t>Discount on commitment</t>
-  </si>
-  <si>
-    <t>Monthly Amount</t>
-  </si>
-  <si>
-    <t>Setup Fees ex. VAT</t>
-  </si>
-  <si>
-    <t>OVHcloud comments:</t>
-  </si>
-  <si>
-    <t>Please refer to the relevant specific conditions of the product/service.</t>
-  </si>
-  <si>
-    <t>Invoice payable at receipt.</t>
-  </si>
-  <si>
-    <t>Invoicing Condition :</t>
-  </si>
-  <si>
-    <t>Terms of payment :</t>
-  </si>
-  <si>
-    <t>Surname, Firstname :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title : </t>
-  </si>
-  <si>
-    <t>Location ……………………………………., date</t>
-  </si>
-  <si>
-    <t>Signature* and stamp</t>
-  </si>
-  <si>
-    <t>*Preceded by the mention "Agreed".</t>
-  </si>
-  <si>
-    <t>Terms &amp; Conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The services are governed exclusively by the following OVHcloud contractual conditions, which can be found here: </t>
-  </si>
-  <si>
-    <t>Our offer is valid for 30 days, subject to product/service availability.</t>
-  </si>
-  <si>
-    <t>AGB Allgemeine Geschäftsbedingungen:</t>
-  </si>
-  <si>
     <t>https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/8ae3988-contrat_genServices-DE-8.3.pdf</t>
   </si>
   <si>
-    <t>https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/912e7a2-OVH_Data_Protection_Agreement-DE-7.1.pdf</t>
+    <t>OVH GmbH, with an authorized capital of € 25.000,  having its registered offfice at  Christophstraße 19, 50670 Köln, Germany registered in Commercial Register Saarbrücken, with the Company Registration Number HRB 15369</t>
   </si>
   <si>
-    <t>Auftragsverarbeitungsvertrag</t>
+    <t>Datum</t>
   </si>
   <si>
-    <t>OVH GmbH, with an authorized capital of € 25.000,  having its registered offfice at  Christophstraße 19, 50670 Köln, Germany registered in Commercial Register Saarbrücken, with the Company Registration Number HRB 15369</t>
+    <t>Referenz</t>
+  </si>
+  <si>
+    <t>Erstellt von</t>
+  </si>
+  <si>
+    <t>Kunde:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zu Händen von: </t>
+  </si>
+  <si>
+    <t>Kontakt:</t>
+  </si>
+  <si>
+    <t>ID:</t>
+  </si>
+  <si>
+    <t>Telefon:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mail: </t>
+  </si>
+  <si>
+    <t>Dienst</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Einrichtungs-gebühr</t>
+  </si>
+  <si>
+    <t>Abrechnungsbedingungen:</t>
+  </si>
+  <si>
+    <t>Zahlungsbedingungen:</t>
+  </si>
+  <si>
+    <t>Informieren Sie sich in den spezifischen Bedingungen des Produkts/Diensts.</t>
+  </si>
+  <si>
+    <t>Rechnung bei Erhalt zahlbar.</t>
+  </si>
+  <si>
+    <t>Dauer / Bindung
+(in Monaten)</t>
+  </si>
+  <si>
+    <t>Rabatt auf Bindung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MONATLICHER GESAMTBETRAG		</t>
+  </si>
+  <si>
+    <t>Einrichtungsgebühr ohne MwSt.</t>
+  </si>
+  <si>
+    <t>Einrichtungsgebühr inkl. MwSt.</t>
+  </si>
+  <si>
+    <t>AGB – Allgemeine Geschäftsbedingungen (Version vom 13.09.2022):</t>
+  </si>
+  <si>
+    <t>https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/231417d-OVH_Data_Protection_Agreement-DE-7.3.pdf</t>
+  </si>
+  <si>
+    <t>Auftragsverarbeitungsvertrag (Version vom 09.08.2023):</t>
+  </si>
+  <si>
+    <t>KUNDE</t>
+  </si>
+  <si>
+    <t>Name, Vorname:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ort ……………………………………., Datum: </t>
+  </si>
+  <si>
+    <t>Unterschrift* und Stempel</t>
+  </si>
+  <si>
+    <t>* Mit der vorangestellten Angabe, Angenommen“</t>
+  </si>
+  <si>
+    <t>Bei Annahme dieses Angebots durch den Kunden werden auch die oben aufgeführten Vertragsbedingungen akzeptiert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gültigkeit des Angebots: </t>
+  </si>
+  <si>
+    <t>30 Tage, Verfügbarkeit vorausgesetzt.</t>
+  </si>
+  <si>
+    <t>MwSt.</t>
+  </si>
+  <si>
+    <t>Dieses Angebot ist vertraulich und darf ohne vorherige schriftliche Genehmigung von OVHcloud weder ganz noch teilweise weitergegeben oder reproduziert werden.</t>
+  </si>
+  <si>
+    <t>Die Anwendbarkeit von Allgemeinen Geschäftsbedingungen oder Kaufbedingungen des Kunden ist ausdrücklich ausgeschlossen. Die Dienste unterliegen ausschließlich den folgenden Vertragsbedingungen von OVHcloud:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angebotsbedingungen </t>
+  </si>
+  <si>
+    <t>Kommentare:</t>
+  </si>
+  <si>
+    <t>If, before the end of the Commitment Period, the Client ceases to use all or part of the Services, the Client will pay to OVHcloud the full price of the Services for the entire Commitment Period. The balance must be paid immediately. In consideration of the Client’s commitment, the discount provided for in this quote will apply on the public prices for the duration of the Commitment Period. “Public prices” means the prices as published on the website of OVHcloud at the time of the Order of the Services. The discounted prices are not cumulative with other discounts, rebates or offers available on the website of OVHcloud. The prices of the Services that are subject to the Commitment Period (discounts included) are firm for the entire Commitment Period. However, the prices of the Services may be changed during the Commitment Period in the event of an increase of the electricity cost and/or the price of the Third-Party Products. If the Client continues to use the Services after the end of the Commitment Period or if the Client orders additional Services, the public prices in force as published on the website of OVHcloud will apply.</t>
   </si>
 </sst>
 </file>
@@ -11194,13 +11210,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="43">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11388,13 +11404,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -11410,12 +11419,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF010F96"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF005EB8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -11480,6 +11483,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF9B9B9B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -11638,7 +11647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -11894,8 +11903,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11926,7 +12089,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11940,57 +12103,44 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="25" borderId="22" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="27" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="17" xfId="57" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
@@ -12002,16 +12152,13 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="33" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="27" fillId="24" borderId="13" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12024,52 +12171,30 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="13" xfId="57" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="47" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="26" borderId="17" xfId="30" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="26" borderId="17" xfId="30" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1"/>
@@ -12088,39 +12213,33 @@
     <xf numFmtId="0" fontId="4" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="38" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="36" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="12" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="12" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="19" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="19" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="47" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -12129,18 +12248,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="57" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="57"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="57"/>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -12168,11 +12279,8 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="40" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="24" borderId="20" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="38" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="24" borderId="20" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12181,47 +12289,138 @@
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="166" fontId="41" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="23" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="24" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="26" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="27" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="28" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="29" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="32" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="62" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="57" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="62" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="28" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="29" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="32" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="35" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="24" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1"/>
-    <xf numFmtId="165" fontId="43" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12229,10 +12428,10 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12244,16 +12443,16 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12271,121 +12470,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="11" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="30" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="1" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="63">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20 % - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="25" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="27" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="31" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Centrify gold" xfId="49" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Entrée" xfId="29" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="42" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="61" builtinId="4"/>
     <cellStyle name="Euro" xfId="30" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Euro 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Euro 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Insatisfaisant" xfId="31" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8"/>
+    <cellStyle name="Explanatory Text" xfId="35" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="33" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="37" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="38" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="39" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="40" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8"/>
+    <cellStyle name="Input" xfId="29" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Milliers 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Milliers 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Milliers 4" xfId="59" xr:uid="{14D347B5-402F-8D41-8897-7199A386B517}"/>
-    <cellStyle name="Monétaire" xfId="61" builtinId="4"/>
     <cellStyle name="Monétaire 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Neutre" xfId="32" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="32" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Normal 2 3" xfId="56" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="Normal 2 3 2" xfId="58" xr:uid="{86FC485C-AE2B-AF43-ADC9-8C2E482CE86C}"/>
+    <cellStyle name="Normal 2 3 2 2 2" xfId="62" xr:uid="{546BAD67-F5BA-7241-AF7F-175E32776264}"/>
     <cellStyle name="Normal 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Note" xfId="28" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="34" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Pourcentage 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Pourcentage 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Pourcentage 3" xfId="55" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Pourcentage 4" xfId="60" xr:uid="{22625C26-9810-C74D-A5AA-B84EE3F92A6B}"/>
-    <cellStyle name="Satisfaisant" xfId="33" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="34" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="35" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="36" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="37" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="38" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="39" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="40" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="36" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -12753,10 +12923,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -12765,7 +12935,7 @@
     <col min="2" max="2" width="72.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
@@ -13341,259 +13511,264 @@
     <col min="16131" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="64"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+    <row r="1" spans="1:13">
+      <c r="A1" s="47"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" ht="20">
-      <c r="A2" s="139" t="s">
+    <row r="2" spans="1:13" ht="20">
+      <c r="A2" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="48"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="5" spans="1:13" ht="14">
+      <c r="C5" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="100"/>
+      <c r="G5" s="108">
+        <f ca="1">NOW()</f>
+        <v>45335.454828587965</v>
+      </c>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="109"/>
+    </row>
+    <row r="6" spans="1:13" ht="55" customHeight="1">
+      <c r="B6" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="102"/>
+      <c r="J6" s="103"/>
+    </row>
+    <row r="7" spans="1:13" ht="14">
+      <c r="A7" s="57"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="105"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="111"/>
+    </row>
+    <row r="8" spans="1:13" ht="14">
+      <c r="C8" s="50">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A9" s="112" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="113"/>
+      <c r="C9" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="141"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="113"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="65"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-    </row>
-    <row r="5" spans="1:10" ht="14">
-      <c r="C5" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="98" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="127">
-        <f ca="1">NOW()</f>
-        <v>45196.822879976855</v>
-      </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
-    </row>
-    <row r="6" spans="1:10" ht="55" customHeight="1">
-      <c r="B6" s="104" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="100" t="s">
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A10" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="J6" s="101"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="67">
+        <v>10</v>
+      </c>
+      <c r="D10" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="117"/>
     </row>
-    <row r="7" spans="1:10" ht="14">
-      <c r="A7" s="74"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="102" t="s">
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="103"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="130"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="67">
+        <v>250</v>
+      </c>
+      <c r="D11" s="118"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="14">
-      <c r="C8" s="67">
+    <row r="12" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="120" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="121"/>
+      <c r="C12" s="67">
+        <v>0</v>
+      </c>
+      <c r="D12" s="106"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="139"/>
+      <c r="C13" s="67">
+        <v>12</v>
+      </c>
+      <c r="D13" s="126"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="128"/>
+      <c r="M13" s="98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="5" customFormat="1" ht="73.5" customHeight="1">
+      <c r="A15" s="133" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="34" t="s">
         <v>20</v>
       </c>
+      <c r="F15" s="80" t="str">
+        <f>"Preis pro Einheit
+"&amp;C5&amp;" ohne MwSt."</f>
+        <v>Preis pro Einheit
+€ ohne MwSt.</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="12" t="str">
+        <f>"Preis "&amp;C5&amp;" ohne MwSt."</f>
+        <v>Preis € ohne MwSt.</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A9" s="131" t="s">
-        <v>16</v>
+    <row r="16" spans="1:13" ht="18" customHeight="1">
+      <c r="A16" s="129" t="s">
+        <v>2</v>
       </c>
-      <c r="B9" s="132"/>
-      <c r="C9" s="68" t="s">
-        <v>5</v>
+      <c r="B16" s="130"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="132"/>
+    </row>
+    <row r="17" spans="1:10" ht="122" customHeight="1">
+      <c r="A17" s="136" t="s">
+        <v>4</v>
       </c>
-      <c r="D9" s="131" t="s">
-        <v>0</v>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="23">
+        <v>10</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="133"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="132"/>
-    </row>
-    <row r="10" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="60" t="s">
+      <c r="F17" s="68">
+        <v>3109</v>
+      </c>
+      <c r="G17" s="24">
         <v>1</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="88">
-        <v>10</v>
-      </c>
-      <c r="D10" s="134" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="136"/>
-    </row>
-    <row r="11" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="88">
-        <v>250</v>
-      </c>
-      <c r="D11" s="137"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="39"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="88">
-        <v>0</v>
-      </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="88">
-        <v>12</v>
-      </c>
-      <c r="D13" s="113"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="114"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="115"/>
-    </row>
-    <row r="15" spans="1:10" s="6" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="120" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="121"/>
-      <c r="C15" s="121"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="18" t="str">
-        <f>"Unit Price "&amp;C5&amp;" ex. VAT/month"</f>
-        <v>Unit Price € ex. VAT/month</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="18" t="str">
-        <f>"Price "&amp;C5&amp;" ex. VAT/month"</f>
-        <v>Price € ex. VAT/month</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="116" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="119"/>
-    </row>
-    <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="123" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="33">
-        <v>10</v>
-      </c>
-      <c r="F17" s="90">
-        <v>3109</v>
-      </c>
-      <c r="G17" s="34">
-        <v>1</v>
-      </c>
-      <c r="H17" s="89">
+      <c r="H17" s="144">
         <v>36</v>
       </c>
-      <c r="I17" s="62">
+      <c r="I17" s="45">
         <v>0.15</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J17" s="46">
         <f>F17*G17*(1-I17)</f>
         <v>2642.65</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="47"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A19" s="44"/>
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A19" s="29"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -13603,191 +13778,190 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A20" s="9"/>
       <c r="B20" s="2"/>
-      <c r="D20" s="81" t="s">
-        <v>23</v>
+      <c r="D20" s="60" t="s">
+        <v>27</v>
       </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="59">
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="44">
         <f>SUM(J17:J17)</f>
         <v>2642.65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="D21" s="83" t="str">
+    <row r="21" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A21" s="9"/>
+      <c r="D21" s="62" t="str">
         <f>C9&amp;" SUPPORT  ("&amp;C10&amp;"% Minimum " &amp; C11&amp;")"</f>
         <v>BUSINESS SUPPORT  (10% Minimum 250)</v>
       </c>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="56">
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="41">
         <f>MAX(0.01*$C$10*J20,$C$11)</f>
         <v>264.26500000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="19" customFormat="1" ht="18" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="83" t="str">
+    <row r="22" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1">
+      <c r="A22" s="9"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="62" t="str">
         <f>IF(C12&gt;0,"Exceptional Discount (-"&amp;C12&amp;"%)","")</f>
         <v/>
       </c>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="56">
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="41">
         <f>(0-J20-J21)*($C$12/100)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="83" t="str">
-        <f>"MONTHLY COST ex. VAT with SUPPORT in "&amp;C6</f>
-        <v>MONTHLY COST ex. VAT with SUPPORT in EURO</v>
+      <c r="A23" s="9"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="62" t="str">
+        <f>"MONATLICHER GESAMTBETRAG ohne MwSt. Inkl. SUPPORT in "&amp;$C$6</f>
+        <v>MONATLICHER GESAMTBETRAG ohne MwSt. Inkl. SUPPORT in EURO</v>
       </c>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="58">
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="43">
         <f>J20+J21+J22</f>
         <v>2906.915</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="83" t="str">
-        <f>"VAT ("&amp;$C$8&amp;"%)"</f>
-        <v>VAT (20%)</v>
+      <c r="A24" s="9"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="62" t="str">
+        <f>"MwSt. ("&amp;$C$8&amp;"%)"</f>
+        <v>MwSt. (19%)</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="108">
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="76">
         <f>$C$8*J23/100</f>
-        <v>581.38300000000004</v>
+        <v>552.31385</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="83" t="s">
-        <v>24</v>
+      <c r="A25" s="9"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="62" t="s">
+        <v>28</v>
       </c>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="20">
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="14">
         <f>SUM(E17:E18)</f>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="20"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:10" s="6" customFormat="1" ht="16" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="D27" s="83" t="str">
-        <f>"Monthly COST including VAT and SUPPORT in "&amp;C6</f>
-        <v>Monthly COST including VAT and SUPPORT in EURO</v>
+    <row r="27" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1">
+      <c r="A27" s="9"/>
+      <c r="D27" s="62" t="str">
+        <f>"MONATLICHER GESAMTBETRAG inkl. MwSt. Inkl. SUPPORT in "&amp;$C$6</f>
+        <v>MONATLICHER GESAMTBETRAG inkl. MwSt. Inkl. SUPPORT in EURO</v>
       </c>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="56">
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="41">
         <f>J23*(1+$C$8/100)</f>
-        <v>3488.2979999999998</v>
+        <v>3459.22885</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="D28" s="83" t="str">
-        <f>"Setup Fees including VAT in "&amp;C6</f>
-        <v>Setup Fees including VAT in EURO</v>
+    <row r="28" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="D28" s="62" t="s">
+        <v>29</v>
       </c>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="56">
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="41">
         <f>J25*(1+$C$8/100)</f>
-        <v>12</v>
+        <v>11.899999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="D29" s="83" t="str">
-        <f>"BUDGET in "&amp;C6&amp;" ex. VAT ("&amp;$C$13&amp;" Months)"</f>
-        <v>BUDGET in EURO ex. VAT (12 Months)</v>
+    <row r="29" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
+      <c r="A29" s="9"/>
+      <c r="D29" s="62" t="str">
+        <f>"Gesamtbudget in "&amp;C6&amp;" ohne MwSt. ("&amp;$C$13&amp;" Monaten)"</f>
+        <v>Gesamtbudget in EURO ohne MwSt. (12 Monaten)</v>
       </c>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="45">
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="30">
         <f>J23*$C$13+J25</f>
         <v>34892.979999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="6" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="D30" s="86" t="str">
-        <f>"BUDGET in "&amp;C6&amp;" including VAT ("&amp;$C$13&amp;" Months) - "&amp;$C$7&amp;" "&amp;$C$8&amp;"%"</f>
-        <v>BUDGET in EURO including VAT (12 Months) - TVA 20%</v>
+    <row r="30" spans="1:10" s="5" customFormat="1" ht="15.5" customHeight="1">
+      <c r="A30" s="9"/>
+      <c r="D30" s="65" t="str">
+        <f>"Gesamtbudget in "&amp;C6&amp;" inkl. MwSt. ("&amp;$C$13&amp;" Monaten) - "&amp;$C$7&amp;" "&amp;$C$8&amp;"%"</f>
+        <v>Gesamtbudget in EURO inkl. MwSt. (12 Monaten) - MwSt. 19%</v>
       </c>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="57">
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="42">
         <f>J29*1.2</f>
         <v>41871.575999999994</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14">
-      <c r="A31" s="11"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A32" s="46"/>
+    <row r="32" spans="1:10" s="5" customFormat="1" ht="14">
+      <c r="A32" s="31"/>
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -13798,500 +13972,328 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="14">
-      <c r="A33" s="27" t="s">
-        <v>25</v>
+      <c r="A33" s="20" t="s">
+        <v>46</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="111"/>
-      <c r="B34" s="112"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31"/>
+      <c r="A34" s="124"/>
+      <c r="B34" s="125"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="87"/>
     </row>
     <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75" t="s">
-        <v>28</v>
+      <c r="A35" s="88"/>
+      <c r="B35" s="89" t="s">
+        <v>21</v>
       </c>
-      <c r="C35" s="77" t="s">
-        <v>26</v>
+      <c r="C35" s="140" t="s">
+        <v>23</v>
       </c>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="78"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="140"/>
+      <c r="J35" s="141"/>
     </row>
     <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76" t="s">
-        <v>29</v>
+      <c r="A36" s="90"/>
+      <c r="B36" s="91" t="s">
+        <v>22</v>
       </c>
-      <c r="C36" s="77" t="s">
-        <v>27</v>
+      <c r="C36" s="142" t="s">
+        <v>24</v>
       </c>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="78"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="142"/>
+      <c r="J36" s="143"/>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="94"/>
+    <row r="37" spans="1:10" ht="15">
+      <c r="A37" s="81"/>
+      <c r="B37" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="84"/>
     </row>
-    <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="91"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="79" t="s">
-        <v>4</v>
+    <row r="38" spans="1:10" ht="14">
+      <c r="A38" s="69"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" ht="21" customHeight="1">
+      <c r="A39" s="73" t="s">
+        <v>45</v>
       </c>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="84"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
     </row>
-    <row r="39" spans="1:10" ht="14">
-      <c r="A39" s="37"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11" t="s">
+    <row r="40" spans="1:10">
+      <c r="A40" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="53"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="109"/>
-      <c r="J39" s="110"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
     </row>
-    <row r="40" spans="1:10" ht="14">
-      <c r="A40" s="37"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
-      <c r="I40" s="109"/>
-      <c r="J40" s="110"/>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
     </row>
-    <row r="41" spans="1:10" ht="14">
-      <c r="A41" s="35"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="11" t="s">
+    <row r="45" spans="1:10">
+      <c r="A45" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="8"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
     </row>
-    <row r="42" spans="1:10" ht="14">
-      <c r="A42" s="32"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="8"/>
+    <row r="47" spans="1:10" ht="14">
+      <c r="A47" s="70"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="26"/>
     </row>
-    <row r="43" spans="1:10" ht="14">
-      <c r="A43" s="37"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="14" t="s">
-        <v>32</v>
+    <row r="48" spans="1:10" ht="84">
+      <c r="A48" s="85" t="str">
+        <f>IF(MAX(H17:H39)&gt;1,"The Client will, as from the time they are made available by OVHcloud, use all the Services specified in this quote during the "&amp; MAX(H17:H39) &amp;" months commitment period (the “Commitment Period”). "&amp; $M$13,"")</f>
+        <v>The Client will, as from the time they are made available by OVHcloud, use all the Services specified in this quote during the 36 months commitment period (the “Commitment Period”). If, before the end of the Commitment Period, the Client ceases to use all or part of the Services, the Client will pay to OVHcloud the full price of the Services for the entire Commitment Period. The balance must be paid immediately. In consideration of the Client’s commitment, the discount provided for in this quote will apply on the public prices for the duration of the Commitment Period. “Public prices” means the prices as published on the website of OVHcloud at the time of the Order of the Services. The discounted prices are not cumulative with other discounts, rebates or offers available on the website of OVHcloud. The prices of the Services that are subject to the Commitment Period (discounts included) are firm for the entire Commitment Period. However, the prices of the Services may be changed during the Commitment Period in the event of an increase of the electricity cost and/or the price of the Third-Party Products. If the Client continues to use the Services after the end of the Commitment Period or if the Client orders additional Services, the public prices in force as published on the website of OVHcloud will apply.</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="8"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="85"/>
     </row>
-    <row r="44" spans="1:10" ht="14">
-      <c r="A44" s="25"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="8"/>
+    <row r="49" spans="1:10">
+      <c r="A49" s="19"/>
+      <c r="C49" s="19"/>
     </row>
-    <row r="45" spans="1:10" ht="14">
-      <c r="A45" s="91"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="11" t="s">
+    <row r="50" spans="1:10" ht="15">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="D50" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="8"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="63"/>
     </row>
-    <row r="46" spans="1:10" ht="14">
-      <c r="A46" s="91"/>
-      <c r="B46" s="92"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="1:10" ht="14">
-      <c r="A47" s="91"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="1:10" ht="14">
-      <c r="A48" s="91"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="1:10" ht="14">
-      <c r="A49" s="91"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="1:10" ht="14">
-      <c r="A50" s="91"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="95"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="1" t="s">
+    <row r="51" spans="1:10" ht="14">
+      <c r="D51" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="122"/>
+      <c r="H51" s="122"/>
+      <c r="I51" s="122"/>
+      <c r="J51" s="123"/>
     </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="5"/>
-      <c r="B52" s="26"/>
+    <row r="52" spans="1:10" ht="14">
+      <c r="D52" s="93"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="122"/>
+      <c r="H52" s="122"/>
+      <c r="I52" s="122"/>
+      <c r="J52" s="123"/>
     </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" ht="21">
-      <c r="A54" s="105" t="s">
+    <row r="53" spans="1:10" ht="14">
+      <c r="D53" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="106"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="107"/>
-      <c r="F54" s="107"/>
-      <c r="G54" s="107"/>
-      <c r="H54" s="107"/>
-      <c r="I54" s="107"/>
-      <c r="J54" s="107"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="6"/>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="69" t="s">
+    <row r="54" spans="1:10" ht="14">
+      <c r="D54" s="94"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:10" ht="14">
+      <c r="D55" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="11"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10" ht="14">
+      <c r="D56" s="95"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="1:10" ht="14">
+      <c r="D57" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="43"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="6"/>
     </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="43"/>
+    <row r="58" spans="1:10" ht="14">
+      <c r="D58" s="94"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="6"/>
     </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="70"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="43"/>
+    <row r="59" spans="1:10" ht="14">
+      <c r="D59" s="94"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="6"/>
     </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B58" s="42"/>
-      <c r="C58" s="43"/>
+    <row r="60" spans="1:10" ht="14">
+      <c r="A60" s="54"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="6"/>
     </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="43"/>
+    <row r="61" spans="1:10" ht="14">
+      <c r="A61" s="56"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="6"/>
     </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="72" t="s">
+    <row r="62" spans="1:10" ht="14">
+      <c r="A62" s="55"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="8"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="56"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="43"/>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="43"/>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="71"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="73"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="43"/>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="72"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="43"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="73"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="43"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="71"/>
-      <c r="B66" s="42"/>
-      <c r="C66" s="43"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="73"/>
-      <c r="B67" s="42"/>
-      <c r="C67" s="43"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="72"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="43"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="73"/>
-      <c r="B69" s="42"/>
-      <c r="C69" s="43"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="71"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="43"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="73"/>
-      <c r="B71" s="42"/>
-      <c r="C71" s="43"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="72"/>
-      <c r="B72" s="42"/>
-      <c r="C72" s="43"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="73"/>
-      <c r="B73" s="42"/>
-      <c r="C73" s="43"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="71"/>
-      <c r="B74" s="42"/>
-      <c r="C74" s="43"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="73"/>
-      <c r="B75" s="42"/>
-      <c r="C75" s="43"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="72"/>
-      <c r="B76" s="42"/>
-      <c r="C76" s="43"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="73"/>
-      <c r="B77" s="42"/>
-      <c r="C77" s="43"/>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="71"/>
-      <c r="B78" s="42"/>
-      <c r="C78" s="43"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="73"/>
-      <c r="B79" s="42"/>
-      <c r="C79" s="43"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="72"/>
-      <c r="B80" s="42"/>
-      <c r="C80" s="43"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="73"/>
-      <c r="B81" s="42"/>
-      <c r="C81" s="43"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="71"/>
-      <c r="B82" s="42"/>
-      <c r="C82" s="43"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="73"/>
-      <c r="B83" s="42"/>
-      <c r="C83" s="43"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="72"/>
-      <c r="B84" s="42"/>
-      <c r="C84" s="43"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="73"/>
-      <c r="B85" s="42"/>
-      <c r="C85" s="43"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="71"/>
-      <c r="B86" s="42"/>
-      <c r="C86" s="43"/>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="73"/>
-      <c r="B87" s="42"/>
-      <c r="C87" s="43"/>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="72"/>
-      <c r="B88" s="42"/>
-      <c r="C88" s="43"/>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="73"/>
-      <c r="B89" s="42"/>
-      <c r="C89" s="43"/>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="71"/>
-      <c r="B90" s="42"/>
-      <c r="C90" s="43"/>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="73"/>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="72"/>
-    </row>
-    <row r="93" spans="1:3" ht="15" customHeight="1">
-      <c r="A93" s="73"/>
-    </row>
-    <row r="94" spans="1:3" ht="15" customHeight="1">
-      <c r="A94" s="71"/>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="73"/>
-    </row>
-    <row r="96" spans="1:3" ht="16" customHeight="1">
-      <c r="A96" s="72"/>
-    </row>
-    <row r="97" spans="1:1" ht="15" customHeight="1">
-      <c r="A97" s="73"/>
-    </row>
-    <row r="98" spans="1:1" ht="15" customHeight="1">
-      <c r="A98" s="71"/>
-    </row>
-    <row r="99" spans="1:1" ht="15" customHeight="1">
-      <c r="A99" s="73"/>
-    </row>
-    <row r="100" spans="1:1" ht="15" customHeight="1">
-      <c r="A100" s="72"/>
-    </row>
-    <row r="101" spans="1:1" ht="15" customHeight="1">
-      <c r="A101" s="73"/>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="71"/>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="73"/>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="72"/>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="73"/>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C36:J36"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14299,88 +14301,23 @@
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:G11"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
-  <phoneticPr fontId="41" type="noConversion"/>
+  <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A61" r:id="rId1" xr:uid="{B64823B1-50BF-1C44-8515-7EEF2938EDB0}"/>
+    <hyperlink ref="A44" r:id="rId1" display="https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/5cec77c-OVH_Data_Protection_Agreement-IE-6.2.pdf" xr:uid="{D9C43030-6FEA-8B4A-B91A-CB46638D67DF}"/>
+    <hyperlink ref="A46" r:id="rId2" display="https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/4789dde-contrat_genServices-IE-7.0.pdf" xr:uid="{418FC6D1-0ED5-F949-9255-11DBB306BE1C}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="69" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="8" scale="69" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14553,6 +14490,68 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14563,24 +14562,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14598,6 +14579,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fixed templates, fixed conformity update bug
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1CFBDC-62E4-9F45-A5F6-0736273C4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4167283B-1709-4F4C-9FB6-99D387B03762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="28800" windowHeight="19060" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quote" sheetId="58" r:id="rId1"/>
@@ -12374,53 +12374,8 @@
     <xf numFmtId="0" fontId="23" fillId="27" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="1" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12476,21 +12431,58 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="30" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="30" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -12925,8 +12917,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13557,13 +13549,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="100"/>
-      <c r="G5" s="108">
+      <c r="G5" s="127">
         <f ca="1">NOW()</f>
-        <v>45335.454828587965</v>
+        <v>45355.528079745367</v>
       </c>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="128"/>
     </row>
     <row r="6" spans="1:13" ht="55" customHeight="1">
       <c r="B6" s="72" t="s">
@@ -13588,10 +13580,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="105"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="111"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="130"/>
     </row>
     <row r="8" spans="1:13" ht="14">
       <c r="C8" s="50">
@@ -13599,98 +13591,98 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="112" t="s">
+      <c r="D9" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="113"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="132"/>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="121"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="67">
         <v>10</v>
       </c>
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="116"/>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="117"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="136"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="121"/>
+      <c r="B11" s="140"/>
       <c r="C11" s="67">
         <v>250</v>
       </c>
-      <c r="D11" s="118"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="121"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="67">
         <v>0</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="139"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="67">
         <v>12</v>
       </c>
-      <c r="D13" s="126"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="127"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="128"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="113"/>
       <c r="M13" s="98" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="133" t="s">
+      <c r="A15" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="135"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="120"/>
       <c r="E15" s="34" t="s">
         <v>20</v>
       </c>
@@ -13715,26 +13707,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="130"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="130"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="132"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="117"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="136" t="s">
+      <c r="A17" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="137"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -13744,7 +13736,7 @@
       <c r="G17" s="24">
         <v>1</v>
       </c>
-      <c r="H17" s="144">
+      <c r="H17" s="106">
         <v>36</v>
       </c>
       <c r="I17" s="45">
@@ -13986,8 +13978,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="124"/>
-      <c r="B34" s="125"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="86"/>
       <c r="D34" s="86"/>
       <c r="E34" s="86"/>
@@ -14002,32 +13994,32 @@
       <c r="B35" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="140" t="s">
+      <c r="C35" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="140"/>
-      <c r="E35" s="140"/>
-      <c r="F35" s="140"/>
-      <c r="G35" s="140"/>
-      <c r="H35" s="140"/>
-      <c r="I35" s="140"/>
-      <c r="J35" s="141"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="141"/>
+      <c r="H35" s="141"/>
+      <c r="I35" s="141"/>
+      <c r="J35" s="142"/>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="90"/>
       <c r="B36" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="142" t="s">
+      <c r="C36" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="142"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="142"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="142"/>
-      <c r="J36" s="143"/>
+      <c r="D36" s="143"/>
+      <c r="E36" s="143"/>
+      <c r="F36" s="143"/>
+      <c r="G36" s="143"/>
+      <c r="H36" s="143"/>
+      <c r="I36" s="143"/>
+      <c r="J36" s="144"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="81"/>
@@ -14156,18 +14148,18 @@
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="122"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="122"/>
-      <c r="J51" s="123"/>
+      <c r="G51" s="107"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107"/>
+      <c r="J51" s="108"/>
     </row>
     <row r="52" spans="1:10" ht="14">
       <c r="D52" s="93"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="122"/>
-      <c r="H52" s="122"/>
-      <c r="I52" s="122"/>
-      <c r="J52" s="123"/>
+      <c r="G52" s="107"/>
+      <c r="H52" s="107"/>
+      <c r="I52" s="107"/>
+      <c r="J52" s="108"/>
     </row>
     <row r="53" spans="1:10" ht="14">
       <c r="D53" s="94" t="s">
@@ -14283,17 +14275,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C36:J36"/>
+  <mergeCells count="18">
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14304,6 +14286,14 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
@@ -14318,6 +14308,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14490,78 +14551,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14577,30 +14593,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed frontend bug with condition and currency symbol
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4167283B-1709-4F4C-9FB6-99D387B03762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12D56D-440B-664E-BD9E-C55AF98F5DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11202,7 +11202,8 @@
     <t>Kommentare:</t>
   </si>
   <si>
-    <t>If, before the end of the Commitment Period, the Client ceases to use all or part of the Services, the Client will pay to OVHcloud the full price of the Services for the entire Commitment Period. The balance must be paid immediately. In consideration of the Client’s commitment, the discount provided for in this quote will apply on the public prices for the duration of the Commitment Period. “Public prices” means the prices as published on the website of OVHcloud at the time of the Order of the Services. The discounted prices are not cumulative with other discounts, rebates or offers available on the website of OVHcloud. The prices of the Services that are subject to the Commitment Period (discounts included) are firm for the entire Commitment Period. However, the prices of the Services may be changed during the Commitment Period in the event of an increase of the electricity cost and/or the price of the Third-Party Products. If the Client continues to use the Services after the end of the Commitment Period or if the Client orders additional Services, the public prices in force as published on the website of OVHcloud will apply.</t>
+    <t>Der Kunde verpflichtet sich, alle Dienste für einen Zeitraum von COMMIT Monaten ab dem Verfügbarkeitsdatum (die "ursprüngliche Vertragslaufzeit") zu nutzen. 
+Wenn der Kunde die Nutzung aller oder eines Teils der Dienste vor Ablauf der ursprünglichen Vertragslaufzeit einstellt, zahlt der Kunde an OVHcloud den vollen Preis für alle Dienste für die gesamte Vertragslaufzeit. Der Restbetrag muss sofort bezahlt werden. Als Gegenleistung für die Verpflichtung des Kunden wird der in diesem Angebot vorgesehene Rabatt auf die öffentlichen Preise für die Dauer der Vertragslaufzeit angewendet. Die "öffentlichen Preise" sind die Preise, die zum Zeitpunkt der Bestellung der Dienste auf der Website von OVHcloud veröffentlicht sind. Die Ermäßigungen sind nicht mit anderen Rabatten, Nachlässen oder Angeboten kumulierbar, die auf der Website von OVHcloud verfügbar sind. Die Preise der Dienste, die der Vertragslaufzeit unterliegen (einschließlich der Rabatte), sind für die gesamte Vertragslaufzeit vereinbart, wobei sich OVHcloud vorbehält die Preise der Dienste während der Vertragslaufzeit im Falle einer Erhöhung der Energiekosten und/oder der Preise von für die Dienste erforderlichen Drittanbieterprodukten (insbesondere Lizenzen) angemessen zu erhöhen. Wenn der Kunde nach der ursprünglichen Vertragslaufzeit weiterhin alle oder einen Teil der Dienste nutzt, sind die zu diesem Zeitpunkt geltenden öffentlichen Preise anwendbar, die auf der Website von OVHcloud veröffentlicht sind, es sei denn, die Parteien haben eine schriftliche Änderung unterzeichnet.</t>
   </si>
 </sst>
 </file>
@@ -11216,7 +11217,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11483,12 +11484,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF9B9B9B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -12354,7 +12349,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="62" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="28" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12376,6 +12370,58 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="30" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12431,58 +12477,9 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="30" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -12917,8 +12914,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13545,17 +13542,17 @@
       <c r="C5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="99" t="s">
+      <c r="E5" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="100"/>
-      <c r="G5" s="127">
+      <c r="F5" s="99"/>
+      <c r="G5" s="112">
         <f ca="1">NOW()</f>
-        <v>45355.528079745367</v>
+        <v>45392.46369016204</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:13" ht="55" customHeight="1">
       <c r="B6" s="72" t="s">
@@ -13564,11 +13561,11 @@
       <c r="C6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="J6" s="103"/>
+      <c r="F6" s="101"/>
+      <c r="J6" s="102"/>
     </row>
     <row r="7" spans="1:13" ht="14">
       <c r="A7" s="57"/>
@@ -13576,14 +13573,14 @@
       <c r="C7" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="105"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="130"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
     </row>
     <row r="8" spans="1:13" ht="14">
       <c r="C8" s="50">
@@ -13591,98 +13588,98 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="131" t="s">
+      <c r="A9" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="131" t="s">
+      <c r="D9" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="133"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="132"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="117"/>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="140"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="67">
         <v>10</v>
       </c>
-      <c r="D10" s="134" t="s">
+      <c r="D10" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="136"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="139" t="s">
+      <c r="A11" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="140"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="67">
         <v>250</v>
       </c>
-      <c r="D11" s="137"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="140"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="67">
         <v>0</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="124"/>
+      <c r="B13" s="143"/>
       <c r="C13" s="67">
         <v>12</v>
       </c>
-      <c r="D13" s="111"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="113"/>
-      <c r="M13" s="98" t="s">
+      <c r="D13" s="130"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="131"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="131"/>
+      <c r="J13" s="132"/>
+      <c r="M13" s="144" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="120"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="139"/>
       <c r="E15" s="34" t="s">
         <v>20</v>
       </c>
@@ -13707,26 +13704,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="115"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="117"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="136"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="121" t="s">
+      <c r="A17" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="122"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="141"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -13736,7 +13733,7 @@
       <c r="G17" s="24">
         <v>1</v>
       </c>
-      <c r="H17" s="106">
+      <c r="H17" s="105">
         <v>36</v>
       </c>
       <c r="I17" s="45">
@@ -13978,8 +13975,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="109"/>
-      <c r="B34" s="110"/>
+      <c r="A34" s="128"/>
+      <c r="B34" s="129"/>
       <c r="C34" s="86"/>
       <c r="D34" s="86"/>
       <c r="E34" s="86"/>
@@ -13994,32 +13991,32 @@
       <c r="B35" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="141" t="s">
+      <c r="C35" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
-      <c r="J35" s="142"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="106"/>
+      <c r="F35" s="106"/>
+      <c r="G35" s="106"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="106"/>
+      <c r="J35" s="107"/>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="90"/>
       <c r="B36" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="143" t="s">
+      <c r="C36" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="143"/>
-      <c r="E36" s="143"/>
-      <c r="F36" s="143"/>
-      <c r="G36" s="143"/>
-      <c r="H36" s="143"/>
-      <c r="I36" s="143"/>
-      <c r="J36" s="144"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="109"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="81"/>
@@ -14108,11 +14105,8 @@
       <c r="B47" s="70"/>
       <c r="C47" s="26"/>
     </row>
-    <row r="48" spans="1:10" ht="84">
-      <c r="A48" s="85" t="str">
-        <f>IF(MAX(H17:H39)&gt;1,"The Client will, as from the time they are made available by OVHcloud, use all the Services specified in this quote during the "&amp; MAX(H17:H39) &amp;" months commitment period (the “Commitment Period”). "&amp; $M$13,"")</f>
-        <v>The Client will, as from the time they are made available by OVHcloud, use all the Services specified in this quote during the 36 months commitment period (the “Commitment Period”). If, before the end of the Commitment Period, the Client ceases to use all or part of the Services, the Client will pay to OVHcloud the full price of the Services for the entire Commitment Period. The balance must be paid immediately. In consideration of the Client’s commitment, the discount provided for in this quote will apply on the public prices for the duration of the Commitment Period. “Public prices” means the prices as published on the website of OVHcloud at the time of the Order of the Services. The discounted prices are not cumulative with other discounts, rebates or offers available on the website of OVHcloud. The prices of the Services that are subject to the Commitment Period (discounts included) are firm for the entire Commitment Period. However, the prices of the Services may be changed during the Commitment Period in the event of an increase of the electricity cost and/or the price of the Third-Party Products. If the Client continues to use the Services after the end of the Commitment Period or if the Client orders additional Services, the public prices in force as published on the website of OVHcloud will apply.</v>
-      </c>
+    <row r="48" spans="1:10">
+      <c r="A48" s="85"/>
       <c r="B48" s="85"/>
       <c r="C48" s="85"/>
       <c r="D48" s="85"/>
@@ -14148,18 +14142,18 @@
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="107"/>
-      <c r="H51" s="107"/>
-      <c r="I51" s="107"/>
-      <c r="J51" s="108"/>
+      <c r="G51" s="126"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="127"/>
     </row>
     <row r="52" spans="1:10" ht="14">
       <c r="D52" s="93"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="107"/>
-      <c r="H52" s="107"/>
-      <c r="I52" s="107"/>
-      <c r="J52" s="108"/>
+      <c r="G52" s="126"/>
+      <c r="H52" s="126"/>
+      <c r="I52" s="126"/>
+      <c r="J52" s="127"/>
     </row>
     <row r="53" spans="1:10" ht="14">
       <c r="D53" s="94" t="s">
@@ -14276,6 +14270,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14286,14 +14288,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
@@ -14308,77 +14302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14551,33 +14474,78 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14593,4 +14561,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed template fr typo
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12D56D-440B-664E-BD9E-C55AF98F5DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE29561-DA6F-8942-B2D6-3E80F20CDBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12375,53 +12375,8 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="31" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="33" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12477,8 +12432,53 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -12914,8 +12914,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13546,13 +13546,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="99"/>
-      <c r="G5" s="112">
+      <c r="G5" s="131">
         <f ca="1">NOW()</f>
-        <v>45392.46369016204</v>
+        <v>45468.523859837966</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="113"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="132"/>
     </row>
     <row r="6" spans="1:13" ht="55" customHeight="1">
       <c r="B6" s="72" t="s">
@@ -13577,10 +13577,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="104"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="115"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="134"/>
     </row>
     <row r="8" spans="1:13" ht="14">
       <c r="C8" s="50">
@@ -13588,98 +13588,98 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="116" t="s">
+      <c r="D9" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="117"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="136"/>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="125"/>
+      <c r="B10" s="144"/>
       <c r="C10" s="67">
         <v>10</v>
       </c>
-      <c r="D10" s="119" t="s">
+      <c r="D10" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="140"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="125"/>
+      <c r="B11" s="144"/>
       <c r="C11" s="67">
         <v>250</v>
       </c>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="125"/>
+      <c r="B12" s="144"/>
       <c r="C12" s="67">
         <v>0</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="142" t="s">
+      <c r="A13" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="143"/>
+      <c r="B13" s="128"/>
       <c r="C13" s="67">
         <v>12</v>
       </c>
-      <c r="D13" s="130"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="131"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="132"/>
-      <c r="M13" s="144" t="s">
+      <c r="D13" s="115"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="117"/>
+      <c r="M13" s="110" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="137" t="s">
+      <c r="A15" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="139"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="124"/>
       <c r="E15" s="34" t="s">
         <v>20</v>
       </c>
@@ -13704,26 +13704,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
-      <c r="A16" s="133" t="s">
+      <c r="A16" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="135"/>
-      <c r="G16" s="135"/>
-      <c r="H16" s="135"/>
-      <c r="I16" s="135"/>
-      <c r="J16" s="136"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="121"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -13975,8 +13975,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="128"/>
-      <c r="B34" s="129"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="114"/>
       <c r="C34" s="86"/>
       <c r="D34" s="86"/>
       <c r="E34" s="86"/>
@@ -14142,18 +14142,18 @@
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="126"/>
-      <c r="H51" s="126"/>
-      <c r="I51" s="126"/>
-      <c r="J51" s="127"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="112"/>
     </row>
     <row r="52" spans="1:10" ht="14">
       <c r="D52" s="93"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="126"/>
-      <c r="H52" s="126"/>
-      <c r="I52" s="126"/>
-      <c r="J52" s="127"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="112"/>
     </row>
     <row r="53" spans="1:10" ht="14">
       <c r="D53" s="94" t="s">
@@ -14270,14 +14270,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14288,6 +14280,14 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
@@ -14302,6 +14302,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14474,78 +14545,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14561,30 +14587,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed template, fixed legal condition
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEC5BD0-6464-E94D-9240-3B1FD2FFD64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB3D19-2586-404E-A770-6D624322B689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11034,7 +11034,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>BUSINESS</t>
   </si>
@@ -11079,9 +11079,6 @@
   </si>
   <si>
     <t>QUOTE</t>
-  </si>
-  <si>
-    <t>https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/8ae3988-contrat_genServices-DE-8.3.pdf</t>
   </si>
   <si>
     <t>OVH GmbH, with an authorized capital of € 25.000,  having its registered offfice at  Christophstraße 19, 50670 Köln, Germany registered in Commercial Register Saarbrücken, with the Company Registration Number HRB 15369</t>
@@ -11149,15 +11146,6 @@
   </si>
   <si>
     <t>Einrichtungsgebühr inkl. MwSt.</t>
-  </si>
-  <si>
-    <t>AGB – Allgemeine Geschäftsbedingungen (Version vom 13.09.2022):</t>
-  </si>
-  <si>
-    <t>https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/231417d-OVH_Data_Protection_Agreement-DE-7.3.pdf</t>
-  </si>
-  <si>
-    <t>Auftragsverarbeitungsvertrag (Version vom 09.08.2023):</t>
   </si>
   <si>
     <t>KUNDE</t>
@@ -12120,7 +12108,7 @@
     <xf numFmtId="164" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
@@ -12341,7 +12329,6 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="62" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="57" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12474,8 +12461,6 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -12908,10 +12893,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13538,45 +13523,45 @@
       <c r="C5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="98" t="s">
-        <v>9</v>
+      <c r="E5" s="97" t="s">
+        <v>8</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="113">
+      <c r="F5" s="98"/>
+      <c r="G5" s="112">
         <f ca="1">NOW()</f>
-        <v>45482.660644791664</v>
+        <v>45583.966796296299</v>
       </c>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="114"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:13" ht="55" customHeight="1">
       <c r="B6" s="72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="100" t="s">
-        <v>10</v>
+      <c r="E6" s="99" t="s">
+        <v>9</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="J6" s="102"/>
+      <c r="F6" s="100"/>
+      <c r="J6" s="101"/>
     </row>
     <row r="7" spans="1:13" ht="14">
       <c r="A7" s="57"/>
       <c r="B7" s="71"/>
       <c r="C7" s="50" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
-      <c r="E7" s="103" t="s">
-        <v>11</v>
+      <c r="E7" s="102" t="s">
+        <v>10</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="116"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
     </row>
     <row r="8" spans="1:13" ht="14">
       <c r="C8" s="50">
@@ -13584,100 +13569,100 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="117" t="s">
-        <v>13</v>
+      <c r="A9" s="116" t="s">
+        <v>12</v>
       </c>
-      <c r="B9" s="118"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="117" t="s">
-        <v>12</v>
+      <c r="D9" s="116" t="s">
+        <v>11</v>
       </c>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="117"/>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="125" t="s">
-        <v>14</v>
+      <c r="A10" s="124" t="s">
+        <v>13</v>
       </c>
-      <c r="B10" s="126"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="67">
         <v>10</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="122"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="125" t="s">
-        <v>15</v>
+      <c r="A11" s="124" t="s">
+        <v>14</v>
       </c>
-      <c r="B11" s="126"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="67">
         <v>250</v>
       </c>
-      <c r="D11" s="123"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="125" t="s">
-        <v>16</v>
+      <c r="A12" s="124" t="s">
+        <v>15</v>
       </c>
-      <c r="B12" s="126"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="67">
         <v>0</v>
       </c>
-      <c r="D12" s="111"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="141" t="s">
-        <v>17</v>
+      <c r="A13" s="140" t="s">
+        <v>16</v>
       </c>
-      <c r="B13" s="142"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="67">
         <v>12</v>
       </c>
-      <c r="D13" s="129"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="130"/>
-      <c r="I13" s="130"/>
-      <c r="J13" s="131"/>
-      <c r="M13" s="110" t="s">
-        <v>47</v>
+      <c r="D13" s="128"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="130"/>
+      <c r="M13" s="109" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="136" t="s">
-        <v>18</v>
+      <c r="A15" s="135" t="s">
+        <v>17</v>
       </c>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="138"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="137"/>
       <c r="E15" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="80" t="str">
         <f>"Preis pro Einheit
@@ -13686,13 +13671,13 @@
 € ohne MwSt.</v>
       </c>
       <c r="G15" s="80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15" s="12" t="str">
         <f>"Preis "&amp;C5&amp;" ohne MwSt."</f>
@@ -13700,26 +13685,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="133"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="134"/>
-      <c r="J16" s="135"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="134"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="139" t="s">
+      <c r="A17" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="140"/>
-      <c r="C17" s="140"/>
-      <c r="D17" s="140"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -13729,7 +13714,7 @@
       <c r="G17" s="24">
         <v>1</v>
       </c>
-      <c r="H17" s="105">
+      <c r="H17" s="104">
         <v>36</v>
       </c>
       <c r="I17" s="45">
@@ -13767,7 +13752,7 @@
       <c r="A20" s="9"/>
       <c r="B20" s="2"/>
       <c r="D20" s="60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="61"/>
       <c r="F20" s="61"/>
@@ -13853,7 +13838,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -13896,7 +13881,7 @@
     <row r="28" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="A28" s="9"/>
       <c r="D28" s="62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -13936,8 +13921,8 @@
       <c r="H30" s="66"/>
       <c r="I30" s="66"/>
       <c r="J30" s="42">
-        <f>J29*1.2</f>
-        <v>41871.575999999994</v>
+        <f>J29*(1+$C$8/100)</f>
+        <v>41522.646199999996</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14">
@@ -13958,7 +13943,7 @@
     </row>
     <row r="33" spans="1:10" ht="14">
       <c r="A33" s="20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -13971,8 +13956,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="127"/>
-      <c r="B34" s="128"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="86"/>
       <c r="D34" s="86"/>
       <c r="E34" s="86"/>
@@ -13985,42 +13970,42 @@
     <row r="35" spans="1:10" ht="15">
       <c r="A35" s="88"/>
       <c r="B35" s="89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
-      <c r="C35" s="106" t="s">
-        <v>23</v>
+      <c r="C35" s="105" t="s">
+        <v>22</v>
       </c>
-      <c r="D35" s="106"/>
-      <c r="E35" s="106"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="106"/>
-      <c r="H35" s="106"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="107"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="105"/>
+      <c r="F35" s="105"/>
+      <c r="G35" s="105"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="106"/>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="90"/>
       <c r="B36" s="91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
-      <c r="C36" s="108" t="s">
-        <v>24</v>
+      <c r="C36" s="107" t="s">
+        <v>23</v>
       </c>
-      <c r="D36" s="108"/>
-      <c r="E36" s="108"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="108"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
-      <c r="J36" s="109"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="107"/>
+      <c r="F36" s="107"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="108"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="81"/>
       <c r="B37" s="82" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37" s="83" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D37" s="83"/>
       <c r="E37" s="83"/>
@@ -14037,7 +14022,7 @@
     </row>
     <row r="39" spans="1:10" ht="21" customHeight="1">
       <c r="A39" s="73" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B39" s="74"/>
       <c r="C39" s="75"/>
@@ -14051,14 +14036,14 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="52" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="53" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
@@ -14068,101 +14053,113 @@
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="92" t="s">
+    <row r="43" spans="1:10" ht="14">
+      <c r="A43" s="70"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="26"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="85"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="85"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="19"/>
+      <c r="C45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" ht="15">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="D46" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="63"/>
+    </row>
+    <row r="47" spans="1:10" ht="14">
+      <c r="D47" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6"/>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" t="s">
-        <v>7</v>
+    <row r="48" spans="1:10" ht="14">
+      <c r="D48" s="92"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="1:10" ht="14">
+      <c r="D49" s="93" t="s">
+        <v>31</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="6"/>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="55" t="s">
+    <row r="50" spans="1:10" ht="14">
+      <c r="D50" s="93"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="1:10" ht="14">
+      <c r="D51" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-    </row>
-    <row r="47" spans="1:10" ht="14">
-      <c r="A47" s="70"/>
-      <c r="B47" s="70"/>
-      <c r="C47" s="26"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="85"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="19"/>
-      <c r="C49" s="19"/>
-    </row>
-    <row r="50" spans="1:10" ht="15">
-      <c r="A50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="19"/>
-      <c r="D50" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="63"/>
-    </row>
-    <row r="51" spans="1:10" ht="14">
-      <c r="D51" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="5"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="143"/>
-      <c r="H51" s="143"/>
-      <c r="I51" s="143"/>
-      <c r="J51" s="144"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10" ht="14">
-      <c r="D52" s="93"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="11"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="143"/>
-      <c r="H52" s="143"/>
-      <c r="I52" s="143"/>
-      <c r="J52" s="144"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:10" ht="14">
-      <c r="D53" s="94" t="s">
-        <v>35</v>
+      <c r="D53" s="93" t="s">
+        <v>33</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="6"/>
     </row>
     <row r="54" spans="1:10" ht="14">
-      <c r="D54" s="94"/>
+      <c r="D54" s="93"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -14171,10 +14168,8 @@
       <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:10" ht="14">
-      <c r="D55" s="95" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="11"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
@@ -14182,8 +14177,11 @@
       <c r="J55" s="6"/>
     </row>
     <row r="56" spans="1:10" ht="14">
-      <c r="D56" s="95"/>
-      <c r="E56" s="11"/>
+      <c r="A56" s="54"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="93"/>
+      <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
@@ -14191,9 +14189,10 @@
       <c r="J56" s="6"/>
     </row>
     <row r="57" spans="1:10" ht="14">
-      <c r="D57" s="94" t="s">
-        <v>37</v>
-      </c>
+      <c r="A57" s="56"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="93"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -14202,65 +14201,23 @@
       <c r="J57" s="6"/>
     </row>
     <row r="58" spans="1:10" ht="14">
-      <c r="D58" s="94"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="6"/>
+      <c r="A58" s="55"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10" ht="14">
-      <c r="D59" s="94"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" ht="14">
-      <c r="A60" s="54"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="94"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" ht="14">
-      <c r="A61" s="56"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="94"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="6"/>
-    </row>
-    <row r="62" spans="1:10" ht="14">
-      <c r="A62" s="55"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="8"/>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="56"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="97" t="s">
-        <v>38</v>
+    <row r="59" spans="1:10">
+      <c r="A59" s="56"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="96" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -14283,18 +14240,64 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A44" r:id="rId1" display="https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/5cec77c-OVH_Data_Protection_Agreement-IE-6.2.pdf" xr:uid="{D9C43030-6FEA-8B4A-B91A-CB46638D67DF}"/>
-    <hyperlink ref="A46" r:id="rId2" display="https://storage.gra.cloud.ovh.net/v1/AUTH_325716a587c64897acbef9a4a4726e38/contracts/4789dde-contrat_genServices-IE-7.0.pdf" xr:uid="{418FC6D1-0ED5-F949-9255-11DBB306BE1C}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="69" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="8" scale="69" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -14303,7 +14306,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14476,7 +14479,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
@@ -14488,57 +14491,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -14546,7 +14507,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14564,7 +14525,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14572,12 +14533,4 @@
     <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixd default zone to empty
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB45864-DF6B-C04A-B027-68460BE8B84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE2627-6298-4D41-BF67-77DAC1B8C75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12126,7 +12126,7 @@
     <xf numFmtId="164" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
@@ -12379,53 +12379,17 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="27" fillId="24" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -12475,18 +12439,53 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="27" fillId="24" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -12923,7 +12922,7 @@
   <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -12932,7 +12931,7 @@
     <col min="2" max="2" width="72.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
@@ -13519,31 +13518,31 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="16"/>
-      <c r="M1" s="139" t="s">
+      <c r="M1" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="139" t="s">
+      <c r="N1" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="139" t="s">
+      <c r="O1" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="139" t="s">
+      <c r="P1" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="139" t="s">
+      <c r="Q1" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="139" t="s">
+      <c r="R1" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="139" t="s">
+      <c r="S1" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="139" t="s">
+      <c r="T1" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="139" t="s">
+      <c r="U1" s="106" t="s">
         <v>51</v>
       </c>
     </row>
@@ -13560,31 +13559,31 @@
       <c r="H2" s="74"/>
       <c r="I2" s="74"/>
       <c r="J2" s="75"/>
-      <c r="M2" s="140" t="s">
+      <c r="M2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="140" t="s">
+      <c r="N2" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="141" t="s">
+      <c r="O2" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="141">
+      <c r="P2" s="108">
         <v>19</v>
       </c>
-      <c r="Q2" s="141" t="s">
+      <c r="Q2" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="142">
+      <c r="R2" s="109">
         <v>10</v>
       </c>
-      <c r="S2" s="142">
+      <c r="S2" s="109">
         <v>250</v>
       </c>
-      <c r="T2" s="142">
+      <c r="T2" s="109">
         <v>12</v>
       </c>
-      <c r="U2" s="142">
+      <c r="U2" s="109">
         <v>0</v>
       </c>
     </row>
@@ -13605,13 +13604,13 @@
         <v>8</v>
       </c>
       <c r="F5" s="94"/>
-      <c r="G5" s="124">
+      <c r="G5" s="112">
         <f ca="1">NOW()</f>
-        <v>45583.988384722223</v>
+        <v>45681.509420949071</v>
       </c>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="125"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:21" ht="55" customHeight="1">
       <c r="B6" s="68" t="s">
@@ -13630,90 +13629,90 @@
         <v>10</v>
       </c>
       <c r="F7" s="99"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="127"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
     </row>
     <row r="9" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="129"/>
-      <c r="D9" s="128" t="s">
+      <c r="B9" s="117"/>
+      <c r="D9" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="129"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="117"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="136" t="s">
+      <c r="A10" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="137"/>
-      <c r="D10" s="131" t="s">
+      <c r="B10" s="125"/>
+      <c r="D10" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="133"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
+      <c r="B11" s="125"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
-      <c r="M11" s="138"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="136" t="s">
+      <c r="A12" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="137"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
+      <c r="B12" s="125"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="120" t="s">
+      <c r="A13" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="121"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110"/>
+      <c r="B13" s="141"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="130"/>
       <c r="M13" s="105" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="115" t="s">
+      <c r="A15" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="117"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="137"/>
       <c r="E15" s="34" t="s">
         <v>19</v>
       </c>
@@ -13738,26 +13737,26 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="18" customHeight="1">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="113"/>
-      <c r="H16" s="113"/>
-      <c r="I16" s="113"/>
-      <c r="J16" s="114"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="134"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -14009,8 +14008,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="106"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="82"/>
       <c r="D34" s="82"/>
       <c r="E34" s="82"/>
@@ -14275,6 +14274,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14285,12 +14290,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -14301,6 +14300,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14473,16 +14481,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14532,19 +14543,15 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14562,23 +14569,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14586,4 +14577,12 @@
     <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed templates col size, added disclaimer
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE2627-6298-4D41-BF67-77DAC1B8C75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69FC6B2-DC9F-FA4B-A686-B6AA93DEC20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12391,6 +12391,54 @@
     <xf numFmtId="2" fontId="27" fillId="24" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12437,54 +12485,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12922,7 +12922,7 @@
   <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -12931,12 +12931,12 @@
     <col min="2" max="2" width="72.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
     <col min="11" max="250" width="11.5" style="1"/>
     <col min="251" max="251" width="10.33203125" style="1" customWidth="1"/>
     <col min="252" max="252" width="87.5" style="1" bestFit="1" customWidth="1"/>
@@ -13604,13 +13604,13 @@
         <v>8</v>
       </c>
       <c r="F5" s="94"/>
-      <c r="G5" s="112">
+      <c r="G5" s="128">
         <f ca="1">NOW()</f>
-        <v>45681.509420949071</v>
+        <v>45701.566173726853</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="113"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
     </row>
     <row r="6" spans="1:21" ht="55" customHeight="1">
       <c r="B6" s="68" t="s">
@@ -13629,90 +13629,90 @@
         <v>10</v>
       </c>
       <c r="F7" s="99"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="115"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="131"/>
     </row>
     <row r="9" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="117"/>
-      <c r="D9" s="116" t="s">
+      <c r="B9" s="133"/>
+      <c r="D9" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="117"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="133"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="125"/>
-      <c r="D10" s="119" t="s">
+      <c r="B10" s="141"/>
+      <c r="D10" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="137"/>
     </row>
     <row r="11" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
+      <c r="B11" s="141"/>
+      <c r="D11" s="138"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="139"/>
+      <c r="G11" s="139"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
+      <c r="B12" s="141"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="141"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="130"/>
+      <c r="B13" s="125"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="114"/>
       <c r="M13" s="105" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="136"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="137"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="121"/>
       <c r="E15" s="34" t="s">
         <v>19</v>
       </c>
@@ -13737,26 +13737,26 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="18" customHeight="1">
-      <c r="A16" s="131" t="s">
+      <c r="A16" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="134"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="118"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="138" t="s">
+      <c r="A17" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="139"/>
-      <c r="C17" s="139"/>
-      <c r="D17" s="139"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -14008,8 +14008,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="126"/>
-      <c r="B34" s="127"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="111"/>
       <c r="C34" s="82"/>
       <c r="D34" s="82"/>
       <c r="E34" s="82"/>
@@ -14274,12 +14274,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14290,6 +14284,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -14300,12 +14300,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14482,15 +14485,12 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14544,9 +14544,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14570,11 +14572,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
apply global discount after support
</commit_message>
<xml_diff>
--- a/static/template_de.xlsx
+++ b/static/template_de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69FC6B2-DC9F-FA4B-A686-B6AA93DEC20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53645DFE-F4AC-0B4C-A983-E4E75DF3EA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12391,6 +12391,54 @@
     <xf numFmtId="2" fontId="27" fillId="24" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -12437,54 +12485,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="29" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="24" borderId="34" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="25" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="36" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="18" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="19" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="20" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="62" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12921,8 +12921,8 @@
   </sheetPr>
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13604,13 +13604,13 @@
         <v>8</v>
       </c>
       <c r="F5" s="94"/>
-      <c r="G5" s="128">
+      <c r="G5" s="112">
         <f ca="1">NOW()</f>
-        <v>45701.566173726853</v>
+        <v>45938.659806365744</v>
       </c>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="129"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:21" ht="55" customHeight="1">
       <c r="B6" s="68" t="s">
@@ -13629,90 +13629,90 @@
         <v>10</v>
       </c>
       <c r="F7" s="99"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="131"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
     </row>
     <row r="9" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="133"/>
-      <c r="D9" s="132" t="s">
+      <c r="B9" s="117"/>
+      <c r="D9" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="133"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="117"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="140" t="s">
+      <c r="A10" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="141"/>
-      <c r="D10" s="135" t="s">
+      <c r="B10" s="125"/>
+      <c r="D10" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="137"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="140" t="s">
+      <c r="A11" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="141"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="139"/>
-      <c r="G11" s="139"/>
+      <c r="B11" s="125"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="140" t="s">
+      <c r="A12" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="127"/>
+      <c r="B12" s="125"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="125"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="114"/>
+      <c r="B13" s="141"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="130"/>
       <c r="M13" s="105" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="119" t="s">
+      <c r="A15" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="121"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="137"/>
       <c r="E15" s="34" t="s">
         <v>19</v>
       </c>
@@ -13737,26 +13737,26 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="18" customHeight="1">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="117"/>
-      <c r="J16" s="118"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="134"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
       <c r="E17" s="23">
         <v>10</v>
       </c>
@@ -13819,8 +13819,8 @@
     <row r="21" spans="1:10" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="A21" s="9"/>
       <c r="D21" s="59" t="str">
-        <f>Q2&amp;" SUPPORT  ("&amp;R2&amp;"% Minimum " &amp; S2&amp;")"</f>
-        <v>BUSINESS SUPPORT  (10% Minimum 250)</v>
+        <f>IF(U2&gt;0,"Exceptional Discount (-"&amp;U2&amp;"%)","")</f>
+        <v/>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="61"/>
@@ -13828,16 +13828,16 @@
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
       <c r="J21" s="41">
-        <f>MAX(0.01*$R$2*J20,$S$2)</f>
-        <v>264.26500000000004</v>
+        <f>(0-J20)*($U$2/100)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="9"/>
       <c r="C22" s="5"/>
       <c r="D22" s="59" t="str">
-        <f>IF(U2&gt;0,"Exceptional Discount (-"&amp;U2&amp;"%)","")</f>
-        <v/>
+        <f>Q2&amp;" SUPPORT  ("&amp;R2&amp;"% Minimum " &amp; S2&amp;")"</f>
+        <v>BUSINESS SUPPORT  (10% Minimum 250)</v>
       </c>
       <c r="E22" s="61"/>
       <c r="F22" s="61"/>
@@ -13845,8 +13845,8 @@
       <c r="H22" s="61"/>
       <c r="I22" s="61"/>
       <c r="J22" s="41">
-        <f>(0-J20-J21)*($U$2/100)</f>
-        <v>0</v>
+        <f>MAX(0.01*$R$2*(0+J20+J21),$S$2)</f>
+        <v>264.26500000000004</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
@@ -14008,8 +14008,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="110"/>
-      <c r="B34" s="111"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="82"/>
       <c r="D34" s="82"/>
       <c r="E34" s="82"/>
@@ -14274,6 +14274,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14284,12 +14290,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -14300,18 +14300,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14484,76 +14531,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14571,18 +14577,12 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>